<commit_message>
updated outputs for f__Atopobiaceae_test_wrapper f__Bacteroidaceae_test_wrapper
</commit_message>
<xml_diff>
--- a/outputs/d__Bacteria_include_p__Firmicutes_A.xlsx
+++ b/outputs/d__Bacteria_include_p__Firmicutes_A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="600" firstSheet="2" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="2" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15880" windowWidth="28800" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="g__Prevotella-t" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="g__C941-t-p" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="f__Lachnospiraceae-t-p" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="g__Ruminococcus_E-t-p" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="f__Atopobiaceae-t" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="f__Bacteroidaceae-t" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -83,21 +85,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -3542,7 +3544,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -5454,7 +5456,4563 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>p__Cyanobacteria</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG440</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-0.3732852661272957</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.860455986454218</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.5937459383035212</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1.743024471677542</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>hRUG890</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.6557150067993616</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2.743497224209109</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.6884188634001576</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.265917456018637</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG836</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1.516019327335052</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1.818232121997508</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.5259364338218117</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.179110907714673</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG025</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2025546442769824</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-5.827318544173674</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1.673655648715718</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.2480414294585193</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG729</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.682957903164596</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-3.571406693015344</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.9709581613407368</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.04605290297303362</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG768</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.776158971414664</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-7.107680550846707</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1.875159704546824</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.377164557356653</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG721</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7334014075846432</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-4.978302178487555</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1.078399425538156</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2.529684058232262</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG161</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.7192720232711824</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-3.798566179317922</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.8427089648039146</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.7493598800678045</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG077</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.281598397292885</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-4.124825158327229</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1.67022903292732</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.2055653041785777</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG725</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.6063788049497301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2.647672677111356</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.7648225736938223</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.892679644650035</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG162</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-1.650995631381004</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-1.556422513910521</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1.321723067176833</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.826822622708564</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG654</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.1689278744153857</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-3.781305532405794</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.478079432603244</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.114318049453061</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>RUG002</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-1.166499500511257</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-2.554334907908526</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1.707748557954199</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.2657815388185606</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>RUG778</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0.3439484710535636</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-1.928417103050202</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.7610543958462364</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.245689148313739</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG032</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.000026453251059</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-3.189862242159927</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.646607894294055</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1.58557191831224</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG001</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1.906881596079779</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-3.9509515508741</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.251249788455183</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-4.055993501591404</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>hRUG864</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.9851323576323496</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.950120258477707</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.4307997498517345</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-2.756466198955647</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG078</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.2527033884515811</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-5.618603084056421</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.9185207971057194</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.8044454077305503</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG004</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.9908973823035365</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-2.643541408889313</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.26664900540704</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-2.603132472408259</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG014</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.232840735113647</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.944917843674683</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1.333324955997464</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-1.899487806346012</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG804</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0.6666815318604979</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-4.04408705406937</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.743579160386309</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.7173847440160257</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>hRUG891</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-1.483466561899275</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-3.266000917880775</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.461854443119036</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-2.314177339458615</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F165"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>p__Cyanobacteria</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG515</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1195640076235608</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-2.566017068976525</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.7960067788937248</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.8498113810895732</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG212</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-2.161153822450005</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2.596893241256609</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.2129934066026379</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1953865710406527</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG062</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.4927365766503566</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2.980394169361479</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.9211965155191838</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1659139260938958</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG419</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-2.768230228360925</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-3.201568372896656</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3399519203449324</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3937426464321007</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>hRUG908</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.165165147235248</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1.937061225145051</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1.387722390824315</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.2035281970356188</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG459</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.2231903358187911</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-3.492958481630628</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1.353285103521143</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.09455960323896712</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG577</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-1.649457813407642</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2.458359367852392</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.3644522398676081</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.2509205185983474</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG112</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.000764076120189</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.160860461738892</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1.08447472879064</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01062419271519578</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG431</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-0.386582052150316</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.524584230870643</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1.717264543260006</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.3102797646275827</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG446</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-1.975797487884835</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1.204636102592214</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.4760280826018662</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.140238870067875</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG318</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-1.113826578179077</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-2.776236897441003</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.6909848307383517</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.1764236251709267</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG483</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.8175924679668825</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-1.335398783700809</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.330027888564936</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.521560668493287</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>RUG838</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-0.6992895973353681</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-1.229935622181299</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1.829612930592945</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.4952357148721037</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>hRUG906</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-3.094402172799485</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.511864996359678</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.05200931095992833</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8083190809008298</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG339</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.05999545413706936</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-1.925877367782803</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-1.424479080848418</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.3868792987937741</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG500</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2432383826764348</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-2.788148004341636</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.5894241969029453</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1.651490674709551</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>RUG273</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.6661780967166422</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-2.984422004475474</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-1.574034241440594</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4732678028386966</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG307</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-1.788470043772151</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.504237815893463</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-2.490141180950185</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.150181475197701</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG397</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.9166543537356657</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-2.53757632692143</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.9429612910987992</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.4136608660323281</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG569</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.6386641550304554</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.646882665134039</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1.459806930490229</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.6520389582697119</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG474</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0.5832826955010129</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-3.492693451292655</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-2.061790070920624</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.2157553051136951</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>hRUG897</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01953784872466102</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-3.557673943079191</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-1.288732066770109</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.3827924520307408</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>RUG116</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-0.6446936320900836</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-2.246258341842143</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.8642409141914154</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.2927752367434142</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>RUG367</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.2914571919395416</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-2.708011366601449</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-0.8020195867729207</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-0.9222341570727456</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>RUG144</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-0.3532840978644143</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-3.06501007633869</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-1.079704262871156</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.1061149691199859</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>RUG423</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.893235788780445</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-3.107230549714153</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.3577066598401933</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.4901346197448612</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>RUG476</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-1.674627940385171</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-1.965807399816344</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-1.31641347234528</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.8389051551624129</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>hRUG858</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-1.258191949447749</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-3.570439786196652</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-1.618556021407958</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.31130956152077</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>RUG168</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1518648937583326</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-2.750190323333756</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-1.470726998504209</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.08013744049484357</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>RUG242</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-0.4699238265626344</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-2.473977798472734</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-0.532355554308144</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-1.36065846790511</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>RUG586</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-2.345698951676201</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-2.714389722503076</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-1.468894129227824</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1.138214567543498</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>RUG106</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-2.088496301943298</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-2.23860317873366</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-1.984417637787688</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.464262233746545</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>RUG765</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.2603189908857657</v>
+      </c>
+      <c r="C34" t="n">
+        <v>-2.764627820192986</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-0.9669994742007979</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.76917449366016</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>RUG259</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-0.4436155627532</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-2.263176177901682</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-1.436653659997289</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.1699119884533771</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>RUG488</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.009857094933801602</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-2.826527797932108</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-2.144956323068044</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.2707583794465195</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>RUG085</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.399025161609127</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-2.967261368332241</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-0.6991441962532059</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.4517860727458856</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>RUG647</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>-1.171590498183679</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-1.783628667387098</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-0.03644750165591226</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.8629502799975336</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>RUG733</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.243002315306125</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-3.110007427204929</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-1.931524364288175</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.6552816642728249</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>RUG064</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-0.2607497751568868</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-2.191508003304961</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-1.250020770488331</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-0.2464864264972528</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>RUG598</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.04773199976793741</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-2.627496345364108</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-0.9717001895926529</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-1.180467437660704</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>RUG022</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-0.8749744763537308</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-2.198602880689301</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-1.758611423274262</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.8717887460981381</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>RUG849</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>-0.17424492754497</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-2.828331995911892</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-2.793440968978151</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.8360231206677684</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>RUG216</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-0.1101760916905843</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-3.151354655345927</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-0.6838883314022792</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.8053099980529486</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>hRUG893</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>-0.9919882226427508</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-1.89069599842511</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-0.387644426734442</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.3721525827096784</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>RUG200</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.1325633420550607</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-1.569948303981475</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-1.813172043754522</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.7187175742646619</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>RUG309</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>-0.2737904370269297</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-3.459273227699771</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-1.495434766184957</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.4785969942393911</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>RUG550</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>-1.028003755478886</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-2.417425598133782</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-0.5839617203055595</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.1956269321463924</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>RUG782</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>-0.8917438173038952</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-1.70953332416624</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-1.662047384528398</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.3338519357854332</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>RUG003</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>-1.369806572086013</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-2.460196420514919</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-0.1487536529738948</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-0.6903062217164511</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>RUG535</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>-0.337506635424337</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-2.11751122654498</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-0.7612781774196864</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-0.2582381233204403</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>RUG315</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.06304563113202816</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-2.623197187110144</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-0.9634796040431164</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.9382603620655187</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>RUG108</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>-0.02444318153859781</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-2.197903498918406</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.5523680231800484</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-1.022835605489743</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>RUG541</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>-0.2843702650470641</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-2.094781407559147</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-0.9436825684797955</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.4702905636263074</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>RUG461</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.5418477751596603</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-2.34381033597052</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-1.031733054983881</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.1679896716913557</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>RUG546</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>-0.71558289359154</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-2.556759146885917</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-2.174348275296719</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.8078540858668084</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="inlineStr">
+        <is>
+          <t>RUG195</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>-0.2424955176766076</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-1.428340702427776</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-0.2428437715641501</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.7280546582437019</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>RUG660</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>-1.311989888224258</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-2.356061326036438</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-0.7477537737817382</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.5905643558649435</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>RUG280</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>-1.556318775102294</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-2.459987652563757</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.655295498065915</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-1.15088883112678</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>RUG614</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.4371794291840231</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-2.185186116919085</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-1.891131230920036</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.8651338905908736</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>RUG742</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.1104476863114346</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-2.583561977457153</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-1.169125963398611</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.08297129991051896</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>RUG457</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>-0.4819822314085747</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-2.398432807622639</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-0.9541295974152733</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.278990203591674</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>RUG036</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>-0.555069042337397</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-1.696413221363012</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-1.394940042473517</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.58501611090992</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>RUG046</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>-0.1582015662295</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-2.251063228238547</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-0.7075860431582242</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.9751084565184318</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>RUG445</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.1826692723303052</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-2.961656951127619</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-1.282294464473682</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.09165198288567759</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>RUG435</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>-0.9911908255693502</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-2.238008558232861</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-1.993593411443041</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.5514400371485265</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>RUG828</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.3163289655459114</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-1.524136731644254</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-1.3609688156208</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.3023394214238869</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>RUG172</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>-0.976162576233883</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-1.666601624206645</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-1.523913502470807</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.1845701500345997</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>RUG589</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>-0.9365985460513724</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-2.002755187149013</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-1.946086101476388</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.7692557147717345</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>RUG169</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.736611088141397</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-2.362918752623347</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-1.70246354031489</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.372133314574114</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>RUG030</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>-0.9933706804769611</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-2.529519359888076</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-0.4567466677370882</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.6531660014297307</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>RUG301</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>-0.3174262168132469</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-3.181021533567588</v>
+      </c>
+      <c r="D72" t="n">
+        <v>-0.3079166420191586</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.368136566758933</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t>hRUG878</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>-2.823125318652998</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-3.821127931593784</v>
+      </c>
+      <c r="D73" t="n">
+        <v>-1.113351057593797</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1.666896519772815</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>RUG037</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>-0.5738987645821616</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-1.676031583859051</v>
+      </c>
+      <c r="D74" t="n">
+        <v>-0.7568906383592902</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-0.4234033912682976</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>RUG711</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>-0.9035598844848776</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-2.913181525923502</v>
+      </c>
+      <c r="D75" t="n">
+        <v>-0.74912348780201</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.08720017428151529</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>RUG788</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>-1.375880997011069</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-3.12590412986466</v>
+      </c>
+      <c r="D76" t="n">
+        <v>-1.276607028078212</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.8526592661388586</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="inlineStr">
+        <is>
+          <t>RUG210</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>-0.2549819030373954</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-1.370026889529413</v>
+      </c>
+      <c r="D77" t="n">
+        <v>-2.358609619189578</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.2538899545511811</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>RUG176</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.1738216312494514</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-2.319403057283796</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-1.505014962318886</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.1786212196859228</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="inlineStr">
+        <is>
+          <t>RUG047</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>-0.7033483885265428</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-3.080331534190923</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-2.027746148858499</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.167432973779194</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>RUG310</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.1021757690305048</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-2.670329340425668</v>
+      </c>
+      <c r="D80" t="n">
+        <v>-1.938122445062898</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-0.2765349147951877</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t>RUG405</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.06912338393259509</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-2.490034409631873</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-1.54281046229704</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.360636900502433</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>hRUG883</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>-0.8098685144689934</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-2.097824176604061</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.2383652134482495</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-1.116525303414053</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>hRUG905</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>-1.180226467979197</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-2.5231779939753</v>
+      </c>
+      <c r="D83" t="n">
+        <v>-1.330395124804742</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.4557298179329375</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>RUG192</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>-1.165462525418429</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-1.810019549964568</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.3533226300753302</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-1.823510533413493</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>RUG697</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>-0.5649817031576287</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-2.481237661553032</v>
+      </c>
+      <c r="D85" t="n">
+        <v>-0.5197437108970693</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-1.162797439041635</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>RUG562</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>-1.438686442328571</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-2.903628033506977</v>
+      </c>
+      <c r="D86" t="n">
+        <v>-2.302299238423952</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.4899872009349286</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>RUG292</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>-1.442180719989877</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-2.859053919069198</v>
+      </c>
+      <c r="D87" t="n">
+        <v>-0.09074944160099685</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-0.6998584899900717</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>RUG376</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>-1.269851068594783</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-1.754605911825901</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.3115015389803677</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-0.6316681732766609</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t>RUG070</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>-1.369443057184384</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-2.605401732901709</v>
+      </c>
+      <c r="D89" t="n">
+        <v>-1.765848746251154</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.965279415388171</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>RUG473</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.1272824078604917</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-3.621349144054122</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-1.810344480835569</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.4707982724400055</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>RUG302</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>-0.2905160818199801</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-2.356942084243785</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-1.727373344080832</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.4451049335647394</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>RUG233</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>-1.298868433469587</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-1.857130745579898</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-1.77077458493319</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-0.8967767720708706</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t>RUG232</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>-0.678556695799726</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-2.065612292506254</v>
+      </c>
+      <c r="D93" t="n">
+        <v>-1.358973720341693</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.1371167093930157</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>RUG207</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>-0.2039992084787885</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-2.991758957042848</v>
+      </c>
+      <c r="D94" t="n">
+        <v>-1.001274340130492</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-0.2709413643918797</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="inlineStr">
+        <is>
+          <t>RUG143</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>-1.203663615469602</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-2.636882660467477</v>
+      </c>
+      <c r="D95" t="n">
+        <v>-0.9804101686586351</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.3167200436551589</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>RUG219</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.08805769478384062</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-2.991020388437548</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-1.7197465889002</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.4117332419465726</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>RUG139</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>-0.3651740908795704</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-2.882609394960495</v>
+      </c>
+      <c r="D97" t="n">
+        <v>-1.310874774473617</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.2055677999710734</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>RUG086</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>-0.7162197463670235</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-2.292508903850881</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-1.844337785133746</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.2184062325441905</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>RUG582</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>-1.452062823511607</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-2.126324799541509</v>
+      </c>
+      <c r="D99" t="n">
+        <v>-0.7855633974428704</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-1.297093055894714</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>RUG418</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>-0.5867612793213282</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-2.163659539793251</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-1.025448981755694</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-0.5681376623044576</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>RUG685</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>-0.02732865791771499</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-2.885272311378513</v>
+      </c>
+      <c r="D101" t="n">
+        <v>-1.214160003260252</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-0.5434800698791087</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>RUG759</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>-1.572578784074921</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-2.429326921956043</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.05646137478393798</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-0.5317099844364715</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>RUG691</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>-0.8503513124336473</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-2.865840524458525</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.1292425999976821</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-0.4123442233722043</v>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>RUG383</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>-0.06578449412081189</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-1.689389171020077</v>
+      </c>
+      <c r="D104" t="n">
+        <v>-0.5298258375340781</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-1.359215685143286</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>RUG056</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>-2.563820510218254</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-2.87579113828431</v>
+      </c>
+      <c r="D105" t="n">
+        <v>-1.200447150197119</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1.041210687561378</v>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>RUG124</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.59535552634321</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-2.087864057549127</v>
+      </c>
+      <c r="D106" t="n">
+        <v>-1.349287307425791</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.326103986293797</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t>RUG160</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0.1957260330402831</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-3.052968302504087</v>
+      </c>
+      <c r="D107" t="n">
+        <v>-0.7874780425516628</v>
+      </c>
+      <c r="E107" t="n">
+        <v>-0.6153717582531971</v>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>RUG624</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>-0.1316545781459904</v>
+      </c>
+      <c r="C108" t="n">
+        <v>-2.573426813921259</v>
+      </c>
+      <c r="D108" t="n">
+        <v>-2.071921418015839</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.44837202786708</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="inlineStr">
+        <is>
+          <t>RUG209</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>-1.182874648518089</v>
+      </c>
+      <c r="C109" t="n">
+        <v>-1.341923832326819</v>
+      </c>
+      <c r="D109" t="n">
+        <v>-2.319219541685603</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.1805570164823123</v>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>RUG812</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>-1.817666136944954</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-1.615462722048021</v>
+      </c>
+      <c r="D110" t="n">
+        <v>-0.8306173376491635</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-0.4650657290413635</v>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="inlineStr">
+        <is>
+          <t>RUG602</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>-0.7215471973660526</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-2.970775763346465</v>
+      </c>
+      <c r="D111" t="n">
+        <v>-0.3593767550671492</v>
+      </c>
+      <c r="E111" t="n">
+        <v>-1.070542519371041</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>RUG751</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>-0.5026688498511045</v>
+      </c>
+      <c r="C112" t="n">
+        <v>-2.300926959402384</v>
+      </c>
+      <c r="D112" t="n">
+        <v>-2.112326344248728</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.3648405237513498</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="inlineStr">
+        <is>
+          <t>RUG101</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>-0.6234270924161704</v>
+      </c>
+      <c r="C113" t="n">
+        <v>-1.962712215473605</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-1.198510079425875</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.08964863624036563</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
+          <t>RUG693</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>0.08384697312554917</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-2.271944530378331</v>
+      </c>
+      <c r="D114" t="n">
+        <v>-0.4896683489826047</v>
+      </c>
+      <c r="E114" t="n">
+        <v>-0.7589019252906715</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="inlineStr">
+        <is>
+          <t>RUG749</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>-1.081818245719967</v>
+      </c>
+      <c r="C115" t="n">
+        <v>-2.518332370521879</v>
+      </c>
+      <c r="D115" t="n">
+        <v>-1.05620071475779</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.4383915967687981</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>RUG107</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>-2.32963205093785</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-1.66577158575339</v>
+      </c>
+      <c r="D116" t="n">
+        <v>-0.6766022461831442</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.3386147570783181</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="inlineStr">
+        <is>
+          <t>RUG063</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0.02416398008542409</v>
+      </c>
+      <c r="C117" t="n">
+        <v>-2.173208954632367</v>
+      </c>
+      <c r="D117" t="n">
+        <v>-0.6366242826491024</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-0.5382788576199745</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="inlineStr">
+        <is>
+          <t>RUG178</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0.1978697142216728</v>
+      </c>
+      <c r="C118" t="n">
+        <v>-3.951576790783003</v>
+      </c>
+      <c r="D118" t="n">
+        <v>-1.59598268696023</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-0.2344199333019148</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="inlineStr">
+        <is>
+          <t>RUG414</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>-1.079084132125785</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-2.268571356744871</v>
+      </c>
+      <c r="D119" t="n">
+        <v>-0.8464165271124062</v>
+      </c>
+      <c r="E119" t="n">
+        <v>-0.08426072018540809</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="inlineStr">
+        <is>
+          <t>RUG058</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>-0.9206090470178721</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-3.110560790068805</v>
+      </c>
+      <c r="D120" t="n">
+        <v>-0.8589505625105945</v>
+      </c>
+      <c r="E120" t="n">
+        <v>-0.9368827648215328</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="inlineStr">
+        <is>
+          <t>RUG771</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0.07852546708492131</v>
+      </c>
+      <c r="C121" t="n">
+        <v>-1.994678260671419</v>
+      </c>
+      <c r="D121" t="n">
+        <v>-1.000232652175316</v>
+      </c>
+      <c r="E121" t="n">
+        <v>-0.3090248420531403</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="inlineStr">
+        <is>
+          <t>RUG837</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>-0.4492801834321205</v>
+      </c>
+      <c r="C122" t="n">
+        <v>-2.999244823313408</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-1.246206993770536</v>
+      </c>
+      <c r="E122" t="n">
+        <v>-0.173847243677798</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="inlineStr">
+        <is>
+          <t>RUG657</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>-0.9808503038071223</v>
+      </c>
+      <c r="C123" t="n">
+        <v>-2.262981853654326</v>
+      </c>
+      <c r="D123" t="n">
+        <v>-0.238470124679172</v>
+      </c>
+      <c r="E123" t="n">
+        <v>-0.0810799457480106</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="inlineStr">
+        <is>
+          <t>RUG174</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>-1.088136708368399</v>
+      </c>
+      <c r="C124" t="n">
+        <v>-2.418808847790538</v>
+      </c>
+      <c r="D124" t="n">
+        <v>-0.9036155370271655</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.3417804551430715</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="inlineStr">
+        <is>
+          <t>RUG355</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>-1.078303217604431</v>
+      </c>
+      <c r="C125" t="n">
+        <v>-2.060604561901775</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-2.093702787977084</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.8001575692838878</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="inlineStr">
+        <is>
+          <t>RUG827</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>-2.760884517791268</v>
+      </c>
+      <c r="C126" t="n">
+        <v>-1.948571896970327</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.02517505118404784</v>
+      </c>
+      <c r="E126" t="n">
+        <v>-1.229128708176857</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="inlineStr">
+        <is>
+          <t>RUG795</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>-0.6426993424497094</v>
+      </c>
+      <c r="C127" t="n">
+        <v>-2.071625552045592</v>
+      </c>
+      <c r="D127" t="n">
+        <v>-1.688323285125836</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.3613206445630563</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="inlineStr">
+        <is>
+          <t>RUG843</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>-1.114672894949546</v>
+      </c>
+      <c r="C128" t="n">
+        <v>-1.419218070032397</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-0.3413292852794947</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-1.883006456500745</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="inlineStr">
+        <is>
+          <t>RUG689</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>-0.3028179178925274</v>
+      </c>
+      <c r="C129" t="n">
+        <v>-2.462307835930459</v>
+      </c>
+      <c r="D129" t="n">
+        <v>-1.216441662552581</v>
+      </c>
+      <c r="E129" t="n">
+        <v>-0.3824796215946102</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="inlineStr">
+        <is>
+          <t>RUG126</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>-0.02143679738621806</v>
+      </c>
+      <c r="C130" t="n">
+        <v>-1.732689966118718</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-1.2322741578226</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-0.3264266098132198</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="inlineStr">
+        <is>
+          <t>RUG451</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>-0.8409247969147358</v>
+      </c>
+      <c r="C131" t="n">
+        <v>-2.634477279200945</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-1.579492827703089</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-0.2291354245237936</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="inlineStr">
+        <is>
+          <t>RUG536</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0.7426122979491396</v>
+      </c>
+      <c r="C132" t="n">
+        <v>-2.602249006664456</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0.06122564637157168</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-1.109271261072697</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="inlineStr">
+        <is>
+          <t>RUG606</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>0.4944652456165821</v>
+      </c>
+      <c r="C133" t="n">
+        <v>-3.882019998043805</v>
+      </c>
+      <c r="D133" t="n">
+        <v>-1.578951328853409</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-0.16046349302199</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="inlineStr">
+        <is>
+          <t>RUG766</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>-0.3093912789017336</v>
+      </c>
+      <c r="C134" t="n">
+        <v>-2.434150060399269</v>
+      </c>
+      <c r="D134" t="n">
+        <v>-0.4468008565112751</v>
+      </c>
+      <c r="E134" t="n">
+        <v>-0.4605715103394391</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="inlineStr">
+        <is>
+          <t>RUG059</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>-0.07652901782804855</v>
+      </c>
+      <c r="C135" t="n">
+        <v>-2.830238521364752</v>
+      </c>
+      <c r="D135" t="n">
+        <v>-0.01007189202137382</v>
+      </c>
+      <c r="E135" t="n">
+        <v>-0.9369336551750969</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="inlineStr">
+        <is>
+          <t>RUG753</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>-0.7533969660764059</v>
+      </c>
+      <c r="C136" t="n">
+        <v>-2.104488863819554</v>
+      </c>
+      <c r="D136" t="n">
+        <v>-0.458002375043208</v>
+      </c>
+      <c r="E136" t="n">
+        <v>-0.7031927246023927</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="inlineStr">
+        <is>
+          <t>RUG744</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>-1.111470835894856</v>
+      </c>
+      <c r="C137" t="n">
+        <v>-1.881670734752835</v>
+      </c>
+      <c r="D137" t="n">
+        <v>-0.8691489677542016</v>
+      </c>
+      <c r="E137" t="n">
+        <v>-0.2855481602874944</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="inlineStr">
+        <is>
+          <t>RUG450</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>-2.287471554478293</v>
+      </c>
+      <c r="C138" t="n">
+        <v>-2.153918509100712</v>
+      </c>
+      <c r="D138" t="n">
+        <v>-0.4425015919067127</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.2154960983010512</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="inlineStr">
+        <is>
+          <t>RUG071</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>-0.6808332526169822</v>
+      </c>
+      <c r="C139" t="n">
+        <v>-2.003264424285603</v>
+      </c>
+      <c r="D139" t="n">
+        <v>-0.5586850345726265</v>
+      </c>
+      <c r="E139" t="n">
+        <v>-0.2121730867325848</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="inlineStr">
+        <is>
+          <t>RUG295</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>-0.8489397720027327</v>
+      </c>
+      <c r="C140" t="n">
+        <v>-1.064588353554654</v>
+      </c>
+      <c r="D140" t="n">
+        <v>-1.367235450149844</v>
+      </c>
+      <c r="E140" t="n">
+        <v>-0.5418582701608079</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="inlineStr">
+        <is>
+          <t>RUG620</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>-0.2521490116745932</v>
+      </c>
+      <c r="C141" t="n">
+        <v>-3.266477993882686</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-1.384635611298445</v>
+      </c>
+      <c r="E141" t="n">
+        <v>-0.365227394637637</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="inlineStr">
+        <is>
+          <t>RUG785</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>-1.067036416644412</v>
+      </c>
+      <c r="C142" t="n">
+        <v>-1.482427643327337</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-1.569553036562022</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0.247940887895043</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="inlineStr">
+        <is>
+          <t>hRUG879</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>-0.7500653325409039</v>
+      </c>
+      <c r="C143" t="n">
+        <v>-2.466477160590266</v>
+      </c>
+      <c r="D143" t="n">
+        <v>-0.613018433312962</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-0.3635418295381604</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="inlineStr">
+        <is>
+          <t>RUG249</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>-1.096604570105696</v>
+      </c>
+      <c r="C144" t="n">
+        <v>-2.971848448341211</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-0.7803652072426946</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0.1986417488018826</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="inlineStr">
+        <is>
+          <t>RUG668</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0.009856011452533342</v>
+      </c>
+      <c r="C145" t="n">
+        <v>-1.961749017611809</v>
+      </c>
+      <c r="D145" t="n">
+        <v>-0.6470466746224652</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-0.4208438420437691</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="inlineStr">
+        <is>
+          <t>RUG430</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>-0.5491968449739937</v>
+      </c>
+      <c r="C146" t="n">
+        <v>-2.559966108497452</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-0.9712229670035741</v>
+      </c>
+      <c r="E146" t="n">
+        <v>-0.6285572886930482</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="inlineStr">
+        <is>
+          <t>RUG424</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>-0.5252130234794887</v>
+      </c>
+      <c r="C147" t="n">
+        <v>-2.772798623824218</v>
+      </c>
+      <c r="D147" t="n">
+        <v>-1.023884549404386</v>
+      </c>
+      <c r="E147" t="n">
+        <v>-0.7257526098017707</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="inlineStr">
+        <is>
+          <t>RUG224</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0.01561702721437097</v>
+      </c>
+      <c r="C148" t="n">
+        <v>-2.531736799225474</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-1.745586991513893</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0.1573357220859438</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="inlineStr">
+        <is>
+          <t>RUG443</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>-0.1373261079781498</v>
+      </c>
+      <c r="C149" t="n">
+        <v>-1.249906805027193</v>
+      </c>
+      <c r="D149" t="n">
+        <v>-2.347010562422993</v>
+      </c>
+      <c r="E149" t="n">
+        <v>-0.5023320460644156</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="inlineStr">
+        <is>
+          <t>RUG136</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>-1.800886364204846</v>
+      </c>
+      <c r="C150" t="n">
+        <v>-3.071719778277081</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-0.7513741538193212</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0.4201969291016409</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="inlineStr">
+        <is>
+          <t>RUG599</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>-0.4615695680951792</v>
+      </c>
+      <c r="C151" t="n">
+        <v>-1.55900940011018</v>
+      </c>
+      <c r="D151" t="n">
+        <v>-1.9580081809731</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.465548956856336</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="inlineStr">
+        <is>
+          <t>hRUG913</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.1211057493512414</v>
+      </c>
+      <c r="C152" t="n">
+        <v>-2.986655882757975</v>
+      </c>
+      <c r="D152" t="n">
+        <v>-0.5812525221460296</v>
+      </c>
+      <c r="E152" t="n">
+        <v>-1.037586645877495</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="inlineStr">
+        <is>
+          <t>RUG204</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>-0.1934641495137072</v>
+      </c>
+      <c r="C153" t="n">
+        <v>-1.434881906381096</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-0.7941214000595227</v>
+      </c>
+      <c r="E153" t="n">
+        <v>-1.097359045694927</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="inlineStr">
+        <is>
+          <t>RUG786</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>-0.5298866333844601</v>
+      </c>
+      <c r="C154" t="n">
+        <v>-1.265368871279055</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-0.8615290830767266</v>
+      </c>
+      <c r="E154" t="n">
+        <v>-0.9107655879656484</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="inlineStr">
+        <is>
+          <t>RUG533</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>-0.7369436603074706</v>
+      </c>
+      <c r="C155" t="n">
+        <v>-2.070552199150397</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-0.4446310507889136</v>
+      </c>
+      <c r="E155" t="n">
+        <v>-0.9348467978588383</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>p__Desulfobacterota</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="inlineStr">
+        <is>
+          <t>RUG413</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>-1.197472599379178</v>
+      </c>
+      <c r="C156" t="n">
+        <v>-1.727379223794557</v>
+      </c>
+      <c r="D156" t="n">
+        <v>-2.118347770655675</v>
+      </c>
+      <c r="E156" t="n">
+        <v>-0.6216541104507851</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="inlineStr">
+        <is>
+          <t>RUG839</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>-1.573744838506864</v>
+      </c>
+      <c r="C157" t="n">
+        <v>-2.043824150390768</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-0.812106460838839</v>
+      </c>
+      <c r="E157" t="n">
+        <v>-0.1552068818298977</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="inlineStr">
+        <is>
+          <t>RUG403</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0.7164664852633731</v>
+      </c>
+      <c r="C158" t="n">
+        <v>-2.61324847640261</v>
+      </c>
+      <c r="D158" t="n">
+        <v>-1.649706044185718</v>
+      </c>
+      <c r="E158" t="n">
+        <v>-0.3096801611889804</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="inlineStr">
+        <is>
+          <t>RUG137</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>-0.5694814646446285</v>
+      </c>
+      <c r="C159" t="n">
+        <v>-2.301604680304857</v>
+      </c>
+      <c r="D159" t="n">
+        <v>-1.357177635692819</v>
+      </c>
+      <c r="E159" t="n">
+        <v>-1.124461387160733</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="inlineStr">
+        <is>
+          <t>RUG504</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>-0.6686334650810559</v>
+      </c>
+      <c r="C160" t="n">
+        <v>-1.916467170300086</v>
+      </c>
+      <c r="D160" t="n">
+        <v>-1.788668550858977</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0.08261210450980928</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="inlineStr">
+        <is>
+          <t>RUG571</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>-1.575687883198123</v>
+      </c>
+      <c r="C161" t="n">
+        <v>-1.804209747711052</v>
+      </c>
+      <c r="D161" t="n">
+        <v>-1.728502606571404</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0.741161307660029</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="inlineStr">
+        <is>
+          <t>RUG317</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>-0.1998082635273715</v>
+      </c>
+      <c r="C162" t="n">
+        <v>-2.378706775379684</v>
+      </c>
+      <c r="D162" t="n">
+        <v>-0.8983892652002181</v>
+      </c>
+      <c r="E162" t="n">
+        <v>-0.3564499270694873</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="inlineStr">
+        <is>
+          <t>RUG815</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>-0.5406720446713971</v>
+      </c>
+      <c r="C163" t="n">
+        <v>-1.102190491904876</v>
+      </c>
+      <c r="D163" t="n">
+        <v>-1.818283335672082</v>
+      </c>
+      <c r="E163" t="n">
+        <v>-0.4004077554971788</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="inlineStr">
+        <is>
+          <t>RUG069</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0.1811153932524325</v>
+      </c>
+      <c r="C164" t="n">
+        <v>-3.096087781762589</v>
+      </c>
+      <c r="D164" t="n">
+        <v>-1.253255792004225</v>
+      </c>
+      <c r="E164" t="n">
+        <v>-0.121729187313414</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>p__Chloroflexota</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="inlineStr">
+        <is>
+          <t>RUG073</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>-1.069645913219906</v>
+      </c>
+      <c r="C165" t="n">
+        <v>-2.76619000337786</v>
+      </c>
+      <c r="D165" t="n">
+        <v>-0.9447100185738297</v>
+      </c>
+      <c r="E165" t="n">
+        <v>-0.258765614333528</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>p__Firmicutes_A</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -6748,7 +11306,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7634,7 +12192,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -10824,7 +15382,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -12262,7 +16820,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -16382,7 +20940,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -18102,7 +22660,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -19278,7 +23836,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -23526,6 +28084,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>